<commit_message>
Finalizada correção e enviado para Colegiado o pedido
</commit_message>
<xml_diff>
--- a/10-planejamento/cronograma/Cronograma-Atividades-Dissertacao.xlsx
+++ b/10-planejamento/cronograma/Cronograma-Atividades-Dissertacao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,33 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>CRONOGRAMA DE ATIVIDADES DISSERTAÇÃO</t>
-  </si>
-  <si>
-    <t>Atividade</t>
-  </si>
-  <si>
-    <t>04/16</t>
-  </si>
-  <si>
-    <t>Mapeamento Sistemático da Literatura</t>
-  </si>
-  <si>
-    <t>Caracterização das Funcionalidades das Ferramentas</t>
-  </si>
-  <si>
-    <t>Pesquisa com Profissionais (Survey)</t>
-  </si>
-  <si>
-    <t>Extensões para as Ferramentas</t>
-  </si>
-  <si>
-    <t>Finalização do texto da dissertação </t>
-  </si>
-  <si>
-    <t>Defesa da dissertação</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">CRONOGRAMA DE ATIVIDADES DISSERTAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atividade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapeamento Sistemático da Literatura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caracterização das Funcionalidades das Ferramentas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pesquisa com Profissionais (Survey)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalização do texto da dissertação </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defesa da dissertação</t>
   </si>
 </sst>
 </file>
@@ -54,7 +51,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/YY"/>
   </numFmts>
   <fonts count="8">
@@ -62,6 +59,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -166,7 +164,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,17 +269,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="10.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,8 +361,8 @@
       <c r="D4" s="6"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -377,12 +375,12 @@
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
@@ -394,12 +392,12 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -410,29 +408,13 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>